<commit_message>
Fix bugs in module 5 template and to protect the sheets
</commit_message>
<xml_diff>
--- a/templates/Module_5_Template.xlsx
+++ b/templates/Module_5_Template.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="14100" tabRatio="391" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="14100" tabRatio="391"/>
   </bookViews>
   <sheets>
     <sheet name="Entry into Labour Market" sheetId="1" r:id="rId1"/>
@@ -3040,8 +3040,8 @@
   <sheetPr codeName="Sheet1"/>
   <dimension ref="A1:CB250"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B5" sqref="B5"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="K4" sqref="K4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.15234375" defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
@@ -3233,9 +3233,7 @@
       <c r="J4" s="5" t="s">
         <v>3</v>
       </c>
-      <c r="K4" s="11">
-        <v>2018</v>
-      </c>
+      <c r="K4" s="11"/>
       <c r="AA4" s="4" t="s">
         <v>15</v>
       </c>
@@ -9923,6 +9921,7 @@
       </c>
     </row>
   </sheetData>
+  <sheetProtection algorithmName="SHA-512" hashValue="68a7xf6NEP5sJK5BnSZRIsPK339oIyGx48io5F4vkImo0bD9tEJ/TGZTetzP0MS+5Hu7s79rpDEP/0bQjWnqng==" saltValue="Qr5iAWaS0E5ibKpfglwrFg==" spinCount="100000" sheet="1" objects="1" scenarios="1"/>
   <mergeCells count="12">
     <mergeCell ref="B1:O1"/>
     <mergeCell ref="B2:O2"/>
@@ -9981,7 +9980,7 @@
   <sheetPr codeName="Sheet2"/>
   <dimension ref="B1:O15"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
+    <sheetView topLeftCell="C1" workbookViewId="0">
       <selection activeCell="I22" sqref="I22"/>
     </sheetView>
   </sheetViews>
@@ -10080,7 +10079,7 @@
       </c>
       <c r="J4" s="6">
         <f>'Entry into Labour Market'!K4</f>
-        <v>2018</v>
+        <v>0</v>
       </c>
       <c r="O4" s="14"/>
     </row>
@@ -10279,6 +10278,7 @@
       <c r="M15" s="10"/>
     </row>
   </sheetData>
+  <sheetProtection algorithmName="SHA-512" hashValue="79PdJ+MgxZ6eLXQObD8hmYPbnqSTtD933mQKSx6KNtXcM47kUYTRQgnM9xX+epAqDfkvalqQ7dTC1EunKJd+qQ==" saltValue="aLY6e0HlEKlHAgbFC0Kztw==" spinCount="100000" sheet="1" objects="1" scenarios="1"/>
   <mergeCells count="11">
     <mergeCell ref="B1:N1"/>
     <mergeCell ref="B2:N2"/>

</xml_diff>